<commit_message>
SH ZSPD new local case
</commit_message>
<xml_diff>
--- a/Mainland CN daily cases by province.xlsx
+++ b/Mainland CN daily cases by province.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HY\Projects\WP_editing\COVID19_provincial_progression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DE09CA-940B-4C96-98F5-1468BD772269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9826E5-7280-44E9-8797-F1A95F401677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{D4D28BB7-1C83-4429-9F12-2BAE470E9B01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{D4D28BB7-1C83-4429-9F12-2BAE470E9B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Hebei" sheetId="1" r:id="rId1"/>
@@ -406,9 +406,6 @@
     <t>http://wsjkw.sh.gov.cn/xwfb/20210204/74fc1b8b797a4d3493e548bdf37934a6.html</t>
   </si>
   <si>
-    <t>last local case: http://wsjkw.sh.gov.cn/xwfb/20210205/c813b32d9b1f4ef0af5f97d14a5a7454.html</t>
-  </si>
-  <si>
     <t>not on provincial health commission site http://wsjkw.km.gov.cn/c/2020-01-22/3267609.shtml</t>
   </si>
   <si>
@@ -507,6 +504,9 @@
   </si>
   <si>
     <t>1st outbreak of year: http://ynswsjkw.yn.gov.cn/wjwWebsite/web/doc/UU161715072535343467</t>
+  </si>
+  <si>
+    <t>last local case until 2 Aug: http://wsjkw.sh.gov.cn/xwfb/20210205/c813b32d9b1f4ef0af5f97d14a5a7454.html</t>
   </si>
 </sst>
 </file>
@@ -21294,8 +21294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1C2ED25-98EE-43A4-81F3-CE756781085A}">
   <dimension ref="A1:I474"/>
   <sheetViews>
-    <sheetView topLeftCell="A449" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:I474"/>
+    <sheetView tabSelected="1" topLeftCell="A449" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H474" sqref="H474"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31881,7 +31881,7 @@
         <v>127</v>
       </c>
       <c r="I383" s="3" t="s">
-        <v>122</v>
+        <v>149</v>
       </c>
     </row>
     <row r="384" spans="1:9" x14ac:dyDescent="0.25">
@@ -46313,7 +46313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{766AC1BC-8EB7-44CF-947D-E657FC340EFE}">
   <dimension ref="A1:I559"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A534" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A534" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A559" sqref="A559"/>
     </sheetView>
   </sheetViews>
@@ -46402,7 +46402,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -46455,7 +46455,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -46484,7 +46484,7 @@
         <v>5</v>
       </c>
       <c r="I6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -46565,7 +46565,7 @@
         <v>26</v>
       </c>
       <c r="I9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -46594,7 +46594,7 @@
         <v>51</v>
       </c>
       <c r="I10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -46623,7 +46623,7 @@
         <v>70</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -46652,7 +46652,7 @@
         <v>80</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -46683,7 +46683,7 @@
         <v>90</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -46714,7 +46714,7 @@
         <v>97</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -46745,7 +46745,7 @@
         <v>106</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -46776,7 +46776,7 @@
         <v>112</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -46805,7 +46805,7 @@
         <v>117</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -46834,7 +46834,7 @@
         <v>123</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -46865,7 +46865,7 @@
         <v>128</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -46896,7 +46896,7 @@
         <v>126</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -46927,7 +46927,7 @@
         <v>123</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -46958,7 +46958,7 @@
         <v>123</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -46989,7 +46989,7 @@
         <v>130</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -47020,7 +47020,7 @@
         <v>134</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -47051,7 +47051,7 @@
         <v>132</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -47082,7 +47082,7 @@
         <v>135</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -47113,7 +47113,7 @@
         <v>133</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -47256,7 +47256,7 @@
         <v>111</v>
       </c>
       <c r="I32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -47933,7 +47933,7 @@
         <v>0</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -47964,7 +47964,7 @@
         <v>1</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -58614,7 +58614,7 @@
         <v>9</v>
       </c>
       <c r="I437" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="438" spans="1:9" x14ac:dyDescent="0.25">
@@ -61305,7 +61305,7 @@
         <v>64</v>
       </c>
       <c r="I533" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="534" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>